<commit_message>
Added Service, Repo and controller for Attr, AttrTypes, User, Seller, Customer, Media, ItemType; Fixed URL naming conventions is rest controllers
</commit_message>
<xml_diff>
--- a/DOCS/ERD Diagram.xlsx
+++ b/DOCS/ERD Diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javawebapp\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CA32AB-5583-4417-910A-A5B974693E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F00F1B4-EB35-468F-BC59-9200E20A5586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{27D5918F-BDF6-4ACF-960F-128FBBC635C4}"/>
   </bookViews>
@@ -363,20 +363,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2626,8 +2622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535F6EF3-832D-4C05-9383-1E2F0AA1D5C6}">
   <dimension ref="A2:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2650,22 +2646,22 @@
       <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2676,16 +2672,16 @@
       <c r="B3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" t="s">
         <v>33</v>
       </c>
       <c r="K3" t="s">
@@ -2702,16 +2698,16 @@
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" t="s">
         <v>1</v>
       </c>
       <c r="K4" t="s">
@@ -2728,12 +2724,12 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="G5" s="5" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="G5" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" t="s">
         <v>6</v>
       </c>
       <c r="K5" t="s">
@@ -2750,10 +2746,10 @@
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" t="s">
         <v>70</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" t="s">
         <v>6</v>
       </c>
       <c r="K6" t="s">
@@ -2770,10 +2766,10 @@
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2818,8 +2814,6 @@
       <c r="E10" t="s">
         <v>1</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
       <c r="K10" t="s">
         <v>71</v>
       </c>
@@ -2828,10 +2822,10 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
@@ -2848,10 +2842,10 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
+      <c r="A12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" t="s">
         <v>33</v>
       </c>
       <c r="D12" t="s">
@@ -2868,10 +2862,10 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
+      <c r="A13" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" t="s">
         <v>1</v>
       </c>
       <c r="D13" t="s">
@@ -2880,10 +2874,10 @@
       <c r="E13" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="5" t="s">
         <v>14</v>
       </c>
       <c r="K13" t="s">
@@ -2894,10 +2888,10 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
+      <c r="A14" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="D14" t="s">
@@ -2920,10 +2914,10 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+      <c r="A15" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" t="s">
         <v>33</v>
       </c>
       <c r="D15" t="s">
@@ -2974,10 +2968,10 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" t="s">
         <v>7</v>
       </c>
       <c r="D18" t="s">
@@ -3000,10 +2994,10 @@
       <c r="H19" t="s">
         <v>14</v>
       </c>
-      <c r="K19" s="7" t="s">
+      <c r="K19" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="L19" s="7" t="s">
+      <c r="L19" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3014,10 +3008,10 @@
       <c r="H20" t="s">
         <v>33</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="K20" t="s">
         <v>38</v>
       </c>
-      <c r="L20" s="5" t="s">
+      <c r="L20" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3028,18 +3022,18 @@
       <c r="H21" t="s">
         <v>1</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="K21" t="s">
         <v>0</v>
       </c>
-      <c r="L21" s="5" t="s">
+      <c r="L21" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G22" t="s">
@@ -3048,18 +3042,18 @@
       <c r="H22" t="s">
         <v>6</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="K22" t="s">
         <v>5</v>
       </c>
-      <c r="L22" s="5" t="s">
+      <c r="L22" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D23" t="s">
@@ -3074,18 +3068,18 @@
       <c r="H23" t="s">
         <v>33</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="K23" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="5" t="s">
+      <c r="L23" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A24" s="5" t="s">
+      <c r="A24" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" t="s">
         <v>33</v>
       </c>
       <c r="D24" t="s">
@@ -3100,18 +3094,18 @@
       <c r="H24" t="s">
         <v>33</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="K24" t="s">
         <v>4</v>
       </c>
-      <c r="L24" s="5" t="s">
+      <c r="L24" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
+      <c r="A25" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" t="s">
         <v>33</v>
       </c>
       <c r="G25" t="s">
@@ -3120,18 +3114,18 @@
       <c r="H25" t="s">
         <v>6</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="K25" t="s">
         <v>21</v>
       </c>
-      <c r="L25" s="5" t="s">
+      <c r="L25" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
+      <c r="A26" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" t="s">
         <v>33</v>
       </c>
       <c r="G26" t="s">
@@ -3140,24 +3134,24 @@
       <c r="H26" t="s">
         <v>7</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="K26" t="s">
         <v>22</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="L26" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
+      <c r="A27" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G27" t="s">
@@ -3166,10 +3160,10 @@
       <c r="H27" t="s">
         <v>7</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="K27" t="s">
         <v>75</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="L27" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3180,17 +3174,16 @@
       <c r="B28" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5" t="s">
+      <c r="D28" t="s">
         <v>46</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K28" s="5" t="s">
+      <c r="E28" t="s">
+        <v>33</v>
+      </c>
+      <c r="K28" t="s">
         <v>23</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="L28" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3201,25 +3194,24 @@
       <c r="B29" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5" t="s">
+      <c r="D29" t="s">
         <v>50</v>
       </c>
-      <c r="E29" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K29" s="5" t="s">
+      <c r="E29" t="s">
+        <v>33</v>
+      </c>
+      <c r="K29" t="s">
         <v>26</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="L29" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D30" s="5" t="s">
+      <c r="D30" t="s">
         <v>29</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" t="s">
         <v>28</v>
       </c>
       <c r="K30" t="s">
@@ -3236,10 +3228,10 @@
       <c r="E31" t="s">
         <v>7</v>
       </c>
-      <c r="G31" s="6" t="s">
+      <c r="G31" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H31" s="6" t="s">
+      <c r="H31" s="5" t="s">
         <v>14</v>
       </c>
       <c r="K31" t="s">
@@ -3270,10 +3262,10 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G33" t="s">
@@ -3336,10 +3328,10 @@
       <c r="H36" t="s">
         <v>85</v>
       </c>
-      <c r="K36" s="6" t="s">
+      <c r="K36" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="L36" s="6" t="s">
+      <c r="L36" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3466,10 +3458,10 @@
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="G44" s="6" t="s">
+      <c r="G44" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="H44" s="6" t="s">
+      <c r="H44" s="5" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>